<commit_message>
need to update the UI and some functionality
</commit_message>
<xml_diff>
--- a/public/templates/export_template.xlsx
+++ b/public/templates/export_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTG_APP\www\Fashion_Asia_Limited\FAL_Commercial\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_file\FAL Commercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5207322D-F35B-4874-B7E3-F9941DBC59B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4FF69F-4F1F-4921-B9F7-390F3E0E1BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="1480" windowWidth="14400" windowHeight="7280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
-    <t>INVOICE No.</t>
-  </si>
-  <si>
-    <t>EXPORT Bill NO.</t>
-  </si>
-  <si>
-    <t>AMOUNT (US$) OF EXPORT GOODS</t>
-  </si>
-  <si>
-    <t>AMOUNT (US$) REALISED</t>
-  </si>
-  <si>
-    <t>G.QTY PCS</t>
-  </si>
-  <si>
-    <t>DATE OF REALISED</t>
-  </si>
-  <si>
-    <t>DUE AMOUNT (US$)</t>
-  </si>
-  <si>
     <t>FAL/ECI/2023-228</t>
   </si>
   <si>
@@ -70,6 +49,27 @@
   </si>
   <si>
     <t>FAL/ECI/2023-235</t>
+  </si>
+  <si>
+    <t>INVOICE No</t>
+  </si>
+  <si>
+    <t>EXPORT Bill NO</t>
+  </si>
+  <si>
+    <t>Realized Value</t>
+  </si>
+  <si>
+    <t>Realized Date</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>DUE AMOUNT</t>
   </si>
 </sst>
 </file>
@@ -80,7 +80,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,16 +103,24 @@
       <scheme val="major"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Calibri Light"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF404040"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -233,63 +241,46 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -609,109 +600,106 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="48.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
+    <row r="1" spans="1:7" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>6</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>17097.7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>16869.59</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>4621</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="4">
         <v>45293</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
         <v>15114.5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>14849.92</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>4085</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>45293</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>29711</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>29314.61</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>8030</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>45293</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="6"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1">
-    <cfRule type="duplicateValues" dxfId="4" priority="5" stopIfTrue="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B1">
     <cfRule type="duplicateValues" dxfId="3" priority="6" stopIfTrue="1"/>
   </conditionalFormatting>
@@ -725,5 +713,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="12" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>